<commit_message>
Auto: Update ETF Data
</commit_message>
<xml_diff>
--- a/data/00981A_Holdings_20260105.xlsx
+++ b/data/00981A_Holdings_20260105.xlsx
@@ -585,10 +585,10 @@
         <v>3196260000</v>
       </c>
       <c r="G6" t="n">
-        <v>-104000</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-168480000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -713,10 +713,10 @@
         <v>2463090000</v>
       </c>
       <c r="G10" t="n">
-        <v>-193000</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>-122362000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -809,10 +809,10 @@
         <v>2298350000</v>
       </c>
       <c r="G13" t="n">
-        <v>-34000</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>-73100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -841,10 +841,10 @@
         <v>2109075000</v>
       </c>
       <c r="G14" t="n">
-        <v>145000</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>221125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -937,10 +937,10 @@
         <v>1902180000</v>
       </c>
       <c r="G17" t="n">
-        <v>209000</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>307230000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1193,10 +1193,10 @@
         <v>560979000</v>
       </c>
       <c r="G25" t="n">
-        <v>-1971000</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>-518373000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1289,10 +1289,10 @@
         <v>373065000</v>
       </c>
       <c r="G28" t="n">
-        <v>157000</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>93415000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1449,10 +1449,10 @@
         <v>249989308.09021</v>
       </c>
       <c r="G33" t="n">
-        <v>-2084000</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>-196521206.3598633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1481,10 +1481,10 @@
         <v>240340000</v>
       </c>
       <c r="G34" t="n">
-        <v>646000</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>157624000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1641,10 +1641,10 @@
         <v>143032500</v>
       </c>
       <c r="G39" t="n">
-        <v>-132000</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>-32274000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1673,10 +1673,10 @@
         <v>91625598.85025024</v>
       </c>
       <c r="G40" t="n">
-        <v>-1060000</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>-64447999.19128418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1961,10 +1961,10 @@
         <v>140500</v>
       </c>
       <c r="G49" t="n">
-        <v>-1738000</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>-244189000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2057,10 +2057,10 @@
         <v>155000</v>
       </c>
       <c r="G52" t="n">
-        <v>-549000</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>-85095000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">

</xml_diff>